<commit_message>
added custom TVAR estimation script aligning with RZ (stata var function) methodology
</commit_message>
<xml_diff>
--- a/Emp_App/RZ_Active_Rep/RZDAT.xlsx
+++ b/Emp_App/RZ_Active_Rep/RZDAT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerchen/Documents/MATLAB/rc_thesis_irf/Emp_App/Ramey_Zubairy_replication_codes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rogerchen/Documents/MATLAB/rc_thesis_irf/Emp_App/RZ_Active_Rep/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB151B3-A32E-A34C-A88F-A3B7B6349AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E4114F-E8A7-494F-92E1-B39DD60C42DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="readme" sheetId="3" r:id="rId1"/>
@@ -1132,9 +1132,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1172,9 +1172,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1207,26 +1207,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1259,26 +1242,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1454,8 +1420,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1717,11 +1683,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AB565"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I7" sqref="I7"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -46122,8 +46088,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:R342"/>
   <sheetViews>
-    <sheetView topLeftCell="A160" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15:R282"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>